<commit_message>
Get daily reddit data: Tue Feb 11 08:10:54 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_16.xlsx
+++ b/data/collected_data/2025_02_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C507"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3508 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1imsri9</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Show me your Valentine’s nails! 🥰💌</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41alvrhtjgie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1imsb9t</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>New builder gel set</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imsb9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ims3y6</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Help please!!</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyiuouq1cgie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1imrd54</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Happy Valentine's!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q769srhq3gie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1imqyix</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>20 minutes, $5 press-on nails, gel glue, and a UV lamp. My lazy girl manicure 🥰</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhtbqobizfie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1imqmwt</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Valentine’s day set 🍓</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imqmwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1imqm52</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Subtle Valentine’s nails🌷</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9v6gp41wfie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1imqjaf</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>What’s the worst experience you’ve ever had at a nail salon?🤔</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k1ff6s7vfie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1imq6h1</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>How can I make my nail beds round instead of square?? I’m really trying to keep up with pushing back my cuticles in a circular motion but they always end up still square looking…</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn057r0prfie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1impra9</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Sonofa ... 😡</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfbhtsxnnfie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1impmy8</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>beetles polish keeps peeling</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1impmy8/beetles_polish_keeps_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1impl80</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Valentine's DIY Set</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1impl80</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1impepw</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Did my boyfriend's nails last night</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1impepw</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1imot04</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>I couldn’t decide what Valentines nail art I wanted so I pick a bunch!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imot04</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1imomcq</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>What’s a normal price for nails</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1imomcq/whats_a_normal_price_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1imojeg</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Valentines Set ❤️💕</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imojeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1imohne</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Valentines day pedicure!!</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imohne</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1imoazu</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Valentine's Nails</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3lfi96gafie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1imnx4r</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Just did this gel x set!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imnx4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1imo67f</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>first time painting my nails in forever</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cz33hroa9fie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1imo0d8</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>first time getting gel extensions. My friend killed it 🩷</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imo0d8</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1imnk3e</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Is this “pocket lifting?”</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imnk3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1imnijj</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Baby pink for my birthday</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7ox1jbq3fie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1immynu</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Valentine nails</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1immynu</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1immtv5</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Valentines Day set ⛓️‍💥🤍💗</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1immtv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1immkfa</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>listened to your advice!!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1immkfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1imm093</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Stupid question about cuticle pushers</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1imm093/stupid_question_about_cuticle_pushers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1imlnmj</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>The Sweetest V Day Nails 🍬🩷</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imlnmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1imlvsy</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Nail broke/split. Should I file it down?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/giprpa4xneie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1imlsqt</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Former nail biter: sad and stressed. Looking for tips</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1imlsqt/former_nail_biter_sad_and_stressed_looking_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1imlq9s</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Soft gel with Half French in pink</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9a5z4qmmeie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1imlmm3</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>tortoise but not? lol</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imlmm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1iml5qa</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Nail biter/picker whose nails are now paper thin after trying dips, acrylics, builder gel</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iml5qa/nail_biterpicker_whose_nails_are_now_paper_thin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1imkerg</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Powerpuff/Valentine's Nails!</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imkerg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1iml34x</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>set i did today</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eodoad49heie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1imkz21</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>New set from today 🎀🪩</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qtztcacgeie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1imkui3</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Pink Strawberry Press-On’s for Valentine’s Day 🍓🩷</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imkui3</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1imkrvh</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Manicure and pedicure for Valentine’s!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imkrvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1imkq8q</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Mardi Gras</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imkq8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1imkg9z</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Happy Vday! ♥️🖤</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jjx0ql0ceie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1imkatc</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>DIY gel nails with 💕</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixy2wbdsaeie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1imk6sp</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>we lost the pinky 😔😔</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imk6sp</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1imk2vv</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>ladybug nails ♥️🐞</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rpd0it809eie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1imjl4c</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Gilded era/tiffany lamp inspired valentine’s nails- I regret my middle finger choice</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imjl4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1imk0qc</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>I like this nail polish on my nails :)</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ajpxykj8eie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1imjlg6</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Want to stop doing dip/acrylic/gel..how to maintain nail strength?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ccxtz385eie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1imjeca</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Valentine Red Cat’s Eye &amp; Lace😍</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmhpf8vn3eie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1imj6bv</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Vday set 🥀✨️❣️</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imj6bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1imj22h</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Sudden allergy to acrylic?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1imj22h/sudden_allergy_to_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1imiwvn</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Matte top coat and no-wipe topcoat</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opk894tyzdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1imiuar</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>is this lifting?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyrxbm2gzdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1imiz8h</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imiz8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1imiwia</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40exbggwzdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1imiq0b</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Valentines nails ❤️💕</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imiq0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1iminhc</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Strawberry shortcake Valentines Day nails! 🍓❤️</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iminhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1imi7o1</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>onyx storm nails ❤️</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vg2wlpruudie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1imi2wo</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dg9jcnywtdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1imi07i</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Perfectly matched manicure</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0e7xp48tdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1imhw30</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Valentines nails with Miffy 🩷</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uo8pfltisdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1imhg9r</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>I'm really loving this color lately</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgazab9bpdie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1imgx6y</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>What is this?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imgx6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1imgnki</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Can you get gel allergy from the paint on solvent/removers?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1imgnki/can_you_get_gel_allergy_from_the_paint_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1imgqfp</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Chrome 🤩✨🪩</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imgqfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1imgn5o</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>diy valentine’s day nails!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxjcwccfjdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1imgdxs</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>First time doing roses</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imgdxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1imgdn4</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>First time playing around with nail decals</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qovacvtghdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1img5s2</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Glue help PLEASE!</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1img5s2/glue_help_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1img834</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Jelly lilac</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ei02xwgcgdie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1img3bq</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Show off your progress! Ive been doing my nails for about a year now and I feel I've made significant progress on my techniques.</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1img3bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1imfy3l</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>What’s wrong with these?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imfy3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1imfxvw</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Nails from Shinjuku!</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imfxvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1imfhyj</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Valentines 🩷❤️</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlh3juz3bdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1imff6f</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Girls HELPPPP what color is simular to this?????</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/637jjbpkadie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1imfcyc</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>I'm in love with this set!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4og0y49adie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1imfaq1</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>my nails grow wide HELP</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1imfaq1/my_nails_grow_wide_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1imf6y4</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Which shape best suites my sausage fingers?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imf6y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1imf5tp</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Feelin’ sweet 💕</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os0ymvos8die1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1imf5ef</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>tried dip powder for the first time!</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imf5ef</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1imf0tr</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>ASP Extra Strength Primer</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stzn08yr7die1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1imeuyw</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>First set done by myself</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imeuyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1imelze</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>My attempt at the stained glass trend! Swipe to see the process 👀</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imelze</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1imemed</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Just seen similar on here, so a different take.</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imemed</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ime90n</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>I tried to do poly gel nails for the first time 😭 how do I improve on application and shaping?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ime90n</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1imdy55</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I do my own 💅🏼</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puix4qh90die1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ime2jc</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Ends chipping</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pugvj821die1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1imdt9x</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Pretty pink nails 💗</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4nmz7vbzcie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1imdoyu</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>happy valentines!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grg6o3igycie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1imdm5c</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Me encantaron ¿Que opinas?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ok0f7uowxcie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1imdi4z</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>feeling like a girl again✨💕</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imdi4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1imdhk8</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>@paintedbycourtney recreation 🖤</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imdhk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1imcw8u</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>first time trying 3d cherries</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imcw8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1im314l</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Did my first nails at home with a dip powder kit !</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1im314l</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1im4nms</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Magnetic cat eye effect kinda disappeared overnight :(</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1im4nms/magnetic_cat_eye_effect_kinda_disappeared/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1im9k85</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Broken nail</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpx5xifw4cie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1imck21</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>When they match your Gameboy</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ninxt0xdqcie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1im8fe6</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Valentine nails</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1im8fe6</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1im91zx</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>I want gel extensions but I want to be able to paint them with regular polish</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1im91zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1im6zio</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Press on nail questions, adhesive tabs vs nail glue etc?</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1im6zio/press_on_nail_questions_adhesive_tabs_vs_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1imbq53</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>I want to put on apres, but I want them short. Is this possible?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1imbq53/i_want_to_put_on_apres_but_i_want_them_short_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1imb4su</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>I don’t know if I love ‘em or hate em</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imb4su</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1imt4cq</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Go Birds</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imt4cq</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1ims2ho</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Holo taco butter me up or mooncat eternal sunshine?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ims2ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1imr8ob</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Star Destroyer</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imr8ob</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1imqzc7</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Does this look bad on me</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imqzc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1imphvq</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>ISO: Nude (beige) base polish with a surprise wild color shimmer, opaque by 3 coats?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imphvq/iso_nude_beige_base_polish_with_a_surprise_wild/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1imper9</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>first cirque order</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9y5t785dkfie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1impddo</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Looking for a color like this, but with purple shimmer</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou6z4li0kfie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1imot5b</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>The most gorgeous green 😍</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g266j02vefie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1imojo7</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Polish that looks like turquoise?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imojo7/polish_that_looks_like_turquoise/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1imne20</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Go Birds!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imne20</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1imna0j</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>How come I’ve never seen a red with a blue shimmer? I feel like that would be so pretty.</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imna0j/how_come_ive_never_seen_a_red_with_a_blue_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1imn68f</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>I have impossible and infuriating nails! Looking for suggestions</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imn68f/i_have_impossible_and_infuriating_nails_looking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1immxzh</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>HELP!</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1immxzh/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1immx75</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Zoya sale ❤️ 2/11 only</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzhuivrzweie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1immoik</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>my favorite color</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdp7ritvueie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1imly3l</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Fun with the DAVIDsTEA collection</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imly3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1imlxlr</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>My roommate laughed at me, I need support. I haven't worn press on nails since the 80s, what kind is good now?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlzfihc5oeie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1imlnsu</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Getting the hang of painting my own nails. 💅</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gexd27r1meie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1imlk76</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>magnetic not velvetizing?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imlk76</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1imk7jp</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Not what I had in mind when I said I was planning on cutting my nails short this week 🥲</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imk7jp</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1imjq4h</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>My brain said “ketchup nails” and I can’t unsee it 😩</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imjq4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1imjodg</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Valentines Mani 2025 #3 - Pahlish, Holo Taco, ILNP</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tkxhqqdu5eie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1imj9d5</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>What I wore in January</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/746rfstl2eie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1imj2vv</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Valentine's Day 💘</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imj2vv</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1imj2ao</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>wearing my first Cracked polish in honor of cracking my thumbnail 😭🤣</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imj2ao</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1imixjc</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>I'm tired of green polish slander!</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bec65q10eie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1imioy9</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Shroomdom 🍄</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imioy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1imie2b</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>(Messy LOL) Holo Taco V-Day Mani</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imie2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1imicvm</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>My Wife Picks My Mani: Part 7</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imicvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1imi1iz</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>It would be great to see an ACLU charity polish or something similar</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imi1iz/it_would_be_great_to_see_an_aclu_charity_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1imhva9</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>My full-hand cat-eye magnet hack</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imhva9</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1imhslp</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>blown AWAY by Dermacol Imperial Rose 02😱</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imhslp</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1imhp26</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Valentines hearts and kisses!</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imhp26</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1imhk57</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Curfew Crasher💜✨️</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imhk57</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1imhj1e</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Polish Pickup exclusive - DRK Nails Nothing to Hide</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imhj1e/polish_pickup_exclusive_drk_nails_nothing_to_hide/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1imh1g5</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Talk me out of it.</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imh1g5</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1imgxub</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imgxub</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1imggf0</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Mildly cat-themed valentine's</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imggf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1imgchh</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Riding Sleeping Bags Down the Stairs</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imgchh</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1img3rq</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>How do I reduce or remove that flap of skin growing onto my nail?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zlf7y2hfdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1img2b7</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Salvaged a disaster</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1img2b7</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1imfa9k</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>💗 a pop of pearl 💗</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imfa9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1imf372</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>What is your favorite Ulta/Sephora/Drug Store base coat without polyvinyl butyral? ORLY bonder has forsaken me.</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imf372/what_is_your_favorite_ultasephoradrug_store_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1imeqey</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Death Valley Nails photo thermals?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imeqey/death_valley_nails_photo_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1imekqc</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Polish dupe for imPRESS Color FX “Fly Up”</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imekqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1imei62</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Update: the mani I did with the "Valentine's" polishes my boyfriend picked</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imei62</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1imefxv</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>"Tenniversary" Nails</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imefxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1imee7i</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>ILNP haul bc i have no self control 😇</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imee7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1imeaj8</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Help! I think this might be cracking? Can I smooth it down with a file?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imeaj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1ime6kw</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Another thermal from Arcana Lacquer. “Gorgon’s Gaze” from the Beyond the Myth collection releasing 2/14 at 6pm EST!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ime6kw</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1ime3gm</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>are holos like impossible to remove or is it ILNP specifically?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ime3gm/are_holos_like_impossible_to_remove_or_is_it_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1imdeud</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>I love macro shots 😍</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/82a25t1gwcie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1imddub</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Swatch request and reviews please for ILNP Poison</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imddub/swatch_request_and_reviews_please_for_ilnp_poison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1imd2kl</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>L.A Color Celestial 😍</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imd2kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1imcjjl</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Fun Valentine Mani 💌💘</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imcjjl</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1imbxv2</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Thinking four shelves would be enough- rookie mistake</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51qyc4evlcie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1imbinm</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Valentines Subterfuge 💖</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1r0kbfzicie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1imb5yf</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Feeling Bold and Blue-tiful!</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imb5yf</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1imaqe3</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Do white polishes stain nails? + Stain prevention tips?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imaqe3/do_white_polishes_stain_nails_stain_prevention/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1imadwt</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Both Holo Taco and Mooncat launching new collections this weekend 😳🫣</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imadwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1imabfg</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>What color are your nails? Yes.</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wfgyya1facie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1ima92n</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Lowkey Blushing 💖</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ima92n</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1im9xiz</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>“Kelpie’s Guise” by Arcana Lacquer! This thermal will be available 2/14 @6pm EST 💚</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1im9xiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1im9w5t</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Swatch and Organization Opinions Plz</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1im9w5t/swatch_and_organization_opinions_plz/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1im9m7s</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>H&amp;M</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ze89m1hb5cie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1im9eat</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Something simple for Valentine’s Day 🎀</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1im9eat</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1im8wrt</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>First timer!</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1im8wrt/first_timer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1im7xn0</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>The main polish for my Valentine's Day mani has the same name as my Valentine 🩷</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ducw7smsbie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1im6w9d</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Dream color combo 😍</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9adxw421kbie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1im6uy5</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Polished for days - Smitten 🦋🪼</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yqutzmhjjbie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1im6a0s</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Pink sheer grey lilac</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1im6a0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1im5ijw</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>I love my hands in this design💞</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s42yz0vq7bie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1im4kb3</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Loving this combo! 😍</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1im4kb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1im468n</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Yes, I love dark nails✨️</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjsv45iotaie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1im3l8q</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1im3l8q/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1im3l8a</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1im3l8a/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1im3gzf</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>ALLERGY TO HEMA PRODUCTS</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1im3gzf/allergy_to_hema_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1im2knr</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Colors not as expected for Cirque Colors Marsala Jelly and Rose Jelly - faulty product or am I just crazy?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1im2knr</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1ilvsda</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Working out with fake nails</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ilvsda/working_out_with_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1ilxw3s</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Help finding 2 swatches?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ilxw3s/help_finding_2_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1imtpky</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Inspired by Wicked. Nails done by Twinkle Nails and Beauty in Melbourne, Australia</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqk0uahwvgie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1imquv0</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Is there a dupe for hard or 3D gel that doesn’t require a UV lamp to set?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1imquv0/is_there_a_dupe_for_hard_or_3d_gel_that_doesnt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1imrmto</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>How do I grow from here?</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imrmto</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1implrk</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>change my nails at least once a week, this is this weeks design!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzxaona7mfie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1imogim</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Valentine’s Day pedi! You</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imogim</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1imlgfx</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Jinx colors with some chains</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imlgfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1imkxa7</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>2000’s vibe?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghqortxwfeie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1imk001</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Did my boyfriend's nails last night</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imk001</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1imj1zl</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Valentine's Day 💞</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imj1zl</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1imilmk</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Cakey cat</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sszflzqnxdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1imig1t</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Love my new nail gal</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imig1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1imh40c</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>New nails 💅🏻💖</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4c3a3rtmdie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1imgo3l</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Mildly cat-themed valentine's</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imgo3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1imfc7j</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Gakuen Handsome Nails for Senior Prom</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1imfc7j/gakuen_handsome_nails_for_senior_prom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1imexew</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Bug set!</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imexew</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1imd4y3</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Valentine’s nails with a twist 🐝🫀</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imd4y3</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1imczpv</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>How do I start?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1imczpv/how_do_i_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1imaonh</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Fiery Valentines nail design♥️</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imaonh</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1ima6hi</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ima6hi/question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1im9i7a</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>How to ensure stable press-ons when doing nail art?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1im9i7a/how_to_ensure_stable_pressons_when_doing_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1im8whe</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Valentines nails (Freehand)</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r57m58tzzbie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1im8b8j</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>snoooooop valentines</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1im8b8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1im5vip</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Beautiful design on short nail</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjxmsw04bbie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1im5oi3</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>I think I took the stained glass nails too far this time 🙈</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjlmhf499bie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1im2yr4</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>another league inspired set</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1im2yr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1im2ge4</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ry7l7fq8aie1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Feb 12 08:10:49 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_16.xlsx
+++ b/data/collected_data/2025_02_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C507"/>
+  <dimension ref="A1:C716"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9052,6 +9052,3559 @@
         </is>
       </c>
     </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1inlby0</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Valentines mani</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inlby0</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1inla2q</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Valentines HK set</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4utlfg5fqnie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1inl67k</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Are you getting valentine nails?</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20yggmn3pnie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1inkv0h</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Slight reset ✨</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inkv0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1inkg9h</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Valentine’s Day cat eye</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gr0yxl0ngnie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1inkdr2</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>v-day nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj2en8ftfnie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1ink1oz</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Strawberry Shortcake nails for February!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ink1oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1injq8c</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>More Valentine’s nails! Powerpuff Girls heart 🩷💞💘</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpx4dj6p8nie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1injo4o</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>CDG inspired nail art ❤️👁️</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1injo4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1inje6u</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>I don’t like these yet</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inje6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1injcvz</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>My mama’s first time doing nail extension</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmu3amfn4nie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1injahn</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Are these bad be honest??!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1injahn</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1inj7qz</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Coffin or almond nails?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inj7qz</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1iniseo</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Would it be weird to order my own nail tips and ask my tech to use them ?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iniseo</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1iniu34</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Cute valentine diy nails ❤️</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eshk3367zmie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1inil5s</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Alright so I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avniuvukwmie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1inicpq</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>is it safe to grow nails out?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inicpq/is_it_safe_to_grow_nails_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1inidjq</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>GOTHIC champagne nails! Feelin fierce</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmdswm7fumie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1ini7sh</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>3 days of soaking and scraping :(</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ini7sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1inhx8o</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Amo</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/he38zo2ypmie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1inht0a</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>gimme butter 🧈🤩</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23pyyaksomie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1inhej2</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Pink glitter</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oa10per1lmie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1inhedv</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Love them❤️</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kxp9je0lmie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1inhe2m</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Builder gel color</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inhe2m/builder_gel_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1inhbmo</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Please help! I've never gotten acrylics before and not sure which would look best.</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inhbmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1inh7i4</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>My nail lady went rogue and I LOVE it</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wkc1vc7jmie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1inh74s</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Raised floral press on nails!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uaa5ezz3jmie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1inh3i7</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>got my nails done today</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k294ia7imie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1ingnpf</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>These nails make me want to dance 🕺🪩</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ingnpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1ingmwp</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>what liquid is used for builder gel?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ingmwp/what_liquid_is_used_for_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1inglte</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>A fresh set to match my energy ✨</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inglte</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1inghlk</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Freestyle</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inghlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1ingf0g</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>gel x [full set] vs acrylic full set [Gel] vs hard gel extension</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ingf0g/gel_x_full_set_vs_acrylic_full_set_gel_vs_hard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1infmi7</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Help with Polygel for Claws :)</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1infmi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1ing2xv</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Wanted to try doing nail designs on myself and did some with a toothpick haha</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ing2xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1ing025</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails 💕</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ing025</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1infvse</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer - For the Love of the Game</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1infvse</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1inffbd</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>What can i use instead if my liquid monomer is finish!!!!!!!!!!!!!!!!!!!!    How long the acrylic nail takes to dry and can u cure it using uv lamp</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inffbd/what_can_i_use_instead_if_my_liquid_monomer_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1inf8i3</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>So shiny, so chrome</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inf8i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1inf24r</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Natural coffin to almond (?)</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inf24r</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1inepp7</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>First time doing a fill on Gel X :)</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6g0iu390xlie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1inep2z</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>My nails for the upcoming second chance prom!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywu8njouwlie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1ineh00</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Valentine 💌💘</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvy04t4xulie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1inecde</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>vintage inspired vday nails! all handpainted</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inecde</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1indxjq</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1indxjq/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1ine8pw</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Like?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1ndrx20tlie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1ine7wt</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Best short nail shape for my hands?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ine7wt</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1ine74g</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>First time overlay</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nfphipmslie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1ine1nc</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Modeling my nails</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ho8oj2sbrlie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1indqe2</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Are these too long? First time trying GelX</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qjxs07qolie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1indaon</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Too much?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1indaon</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1ind4kn</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Valentines Day nails I did myself</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tir311tqjlie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1incxsm</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>The nail tech drilled through my nail — I’m literally crying in the nail salon</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1incxsm/the_nail_tech_drilled_through_my_nail_im/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1incwzo</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>My manicurist told me that the baby boomer looks better in acrylics than with any other technique. Is this true?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3d0jk310ilie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1incgz6</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Simple Set for Valentine’s❤️</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1incgz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1incfd5</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Valentine nails 🩷 pink with white chrome, I loveee</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gej9fn4elie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1inc9mq</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Fresh fill.. I love this chrome!</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od9bioruclie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1inc7c0</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Hand painted &amp; sculpted vday set💕</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inc7c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1inc4r1</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>first time getting cat eye nails and obsessed is an understatement! 💗</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eutujjatblie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1inc32j</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Maybe my favorite set EVER 😍</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4pmc47fblie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1inc2wd</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Glowing Nails 😍</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inc2wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1inbxo6</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Valentine’s Set 🎀💖💋🍬</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nqlply7alie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1inbrsv</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Are these wonky or am I picky?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gu0itcry8lie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1inb825</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Gel X glued with regular nail glue</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inb825/gel_x_glued_with_regular_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1inbr0e</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>How's the blue?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqyicajs8lie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1inbqic</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Cute little shroomies this month!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxyxegto8lie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1inbldc</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Ready for Valentine's</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlvf62gl7lie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1inb70r</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>A few days ago I made this design, what do you think?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgxgobpn4lie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1inavkk</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Question about nail set sizes</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inavkk/question_about_nail_set_sizes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1in9bsw</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Natural Nails under Gel Nails</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1in9bsw/natural_nails_under_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1in9gh6</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Contact dermatitis ?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in9gh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1ina0v1</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>I love my Valentine's Day nails!!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3m66xbyvkie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1in9srm</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Color Turned Out Better Than I Expected</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3ugafsaukie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1in9qb9</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>French manicure colour: Rosé on ice</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ffohf4ttkie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1in9lo7</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>wanted to post my fav set so far!</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bffyiguwskie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1in9i84</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Do you prefer gels or regular for pedicure?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1in9i84/do_you_prefer_gels_or_regular_for_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1in8rpw</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>My girl Jocelyn did it again 💜🤩</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in8rpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1in8jqn</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Love Hūrts Movie Nails</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in8jqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1in8jhq</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Basecoat without a strengthener</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1in8jhq/basecoat_without_a_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1in8e6u</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Fresh set!</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yn4dez42kkie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1in7shj</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Candy heart Valentine’s nails! (done by divabeauty_nailspa on Instagram) &lt;3</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in7shj</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1in7rm3</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Yes....Yes I did- Vday nails</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in7rm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1in769n</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Of course, V-day nails :)</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr9y7ms5bkie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1in73lu</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Proximal nail fold (?) on my left thumb always gets dry and crusty like this, always on the same side, too - I use cuticle oil and creams every few days but it still recurs. Never happens to my other fingers. What’s the cause? What can I do?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7dvnn2nakie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1in6wof</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day Mani</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in6wof</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1in63lx</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Girlie pop nails 🎀💖✨</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in63lx</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1in5ork</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>When your left hand came out like this, and you still have to do your right hand, with your right hand. Pressure.</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in5ork</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1in5pfk</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Valentine’s nails :)</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in5pfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1in5lrf</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Simple valentine set</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in5lrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1in5dx1</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Press ons are ruining my nails?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1in5dx1/press_ons_are_ruining_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1in5gtd</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>overgrowth of skin under nails?</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in5gtd</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1in410n</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in410n</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1in4p57</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>❤️🖤</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5bi552htjie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1in45s9</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>new claws ❤️</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in45s9</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1in4058</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Long time lurker. Please rate my beginner nails.</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9lue1igojie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1in38fs</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Pretty simple, but I like it ❤️</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in38fs</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1in32js</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>At Home Builder Gel Advice</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1in32js/at_home_builder_gel_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1in2ppi</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Love a good red💋</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in2ppi</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1in1nu2</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Valentine's nail art</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in1nu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1in1j39</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Chipped dip fix?</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1in1j39/chipped_dip_fix/</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1inkxbm</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>How to remove gel from underneath fingertips?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1inkxbm/how_to_remove_gel_from_underneath_fingertips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1inktgg</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Slight refresh 💖</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inktgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ink8cs</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Played with power tools and installed shelves for all my polishes…And it’s already full</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/verhubx5enie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ink4j2</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Purple, black and a be - glittered cat 😂🤷‍♀️</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/wN14Dmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1ink1jz</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Pink velvet nails 💖</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ink1jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1injdw2</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Is this salvageable?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1injdw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1injboy</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Accidental Wicked Nails</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3l1t5cc4nie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1inj15c</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>I guess 3+ hours wasn’t enough drying time 🥲</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uhap82a1nie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1iniort</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>kb shimmer recs</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wfne85gnxmie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1iniep9</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Just spilled half a bottle of base coat all over my floor</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iniep9/just_spilled_half_a_bottle_of_base_coat_all_over/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1ini9a4</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>It’s Glo Time</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ini9a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1inho4l</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Abomination vs. Essie</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inho4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1inh3z0</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Classic Cherry but make it Valentine's</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inh3z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1inh0n2</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>New nail shape just dropped (jumpscare warning/NOT my nails)</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dy304mmghmie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1ingqka</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>BKL Goddess of Rot vs ILNP Penny?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ingqka/bkl_goddess_of_rot_vs_ilnp_penny/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1ingo6w</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Happy 59th Momma. I got a top coat on mine, I bough her new set 😌🎂🥳🎊🎁💅</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ingo6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1infyof</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>OMG YOU GUYS LOOK!!</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1infyof</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1infv42</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>For the Love of the Game</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1infv42</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1inftkq</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Bees knees lacquer 20% off sale 2/21</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoip4fbk6mie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1infem8</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>I tried the heart magnetic polish hack and it didn't work at all lol</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yevqi5ax2mie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1inex0k</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Moo~</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inex0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1ines4k</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Any ingredients other than polyvinyl butyral that can cause nail peeling?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ines4k/any_ingredients_other_than_polyvinyl_butyral_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1ineqkp</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>My Valentine checking out my Valentine's week manicure</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ineqkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1inefko</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Venetian Charm</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inefko</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1ine5xp</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Does anyone have sensitive skin and still use gel polish?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ine5xp/does_anyone_have_sensitive_skin_and_still_use_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1ine3ch</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Norpsilocin + psilocin 🍄🤯</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oljm6zhqrlie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1indxrk</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>twisted terracotta tanzanite</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1indxrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1indotw</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>I may have overdone it with the glitter…</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgueat8dolie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1indgpm</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Pink Velvet 💕</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1indgpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1ind82h</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Bramble and Burr</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ind82h</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1incwnx</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Valentine’s Day skittle featuring (mostly) Mooncat</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1incwnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1inct51</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Nails I did for valentines!</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ett702i6hlie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1inceby</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Easy Valentine’s nail inspo: pink glitter bomb to blind your valentine 💖💅</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inceby</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1inca3l</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>No Child Hungry 🩵</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inca3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1inc1tn</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>How to get thin coats?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1inc1tn/how_to_get_thin_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1inbsnw</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Nails are like thin plastic</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1inbsnw/nails_are_like_thin_plastic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1inblzt</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Monster Nails 💜</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wm9a4knerjie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1inbk2q</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>✨💚PFD Airy🩷✨</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yq520pdb7lie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1ina3ph</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Be my Valentine ❤️</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2itffsiwkie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1in9v8i</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Help! I can’t stop staring at my nails!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in9v8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1in9rfv</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Chrome nails, pré top coat</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crib2vr0ukie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1in9hsh</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Had no idea ILNP Joy was so juicy 😍</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in9hsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1in8re9</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Red smooth velvet lacquer</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/taw46slqmkie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1in7bf8</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>strawberries and cream 🍓🍦✨</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khb5ykm6ckie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1in79er</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Meet my ‘Mystery Skittle Bins’</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in79er</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1in6x28</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>I can't with this packaging</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in6x28</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1in5xhh</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>New at this</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1in5xhh/new_at_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1in5i6p</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>How to fix nails</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in5i6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1in4yl0</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Enjoying snowy days with thermals!</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in4yl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1in4xxz</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Feeling a Little Matte</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxodn557vjie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1in4afv</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>THANK YOU!!!!</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in4afv</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1in3vlo</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Clionadh favorites</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in3vlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1in3m35</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Minimalist art</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in3m35</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1in2vgw</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>First (successful) attempt at heart tips 💕</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in2vgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1in2gjw</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Accidentally on purpose?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in2gjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1in2fg7</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>First Time Trying Fluid Art Nails ❤️🩷❤️</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in2fg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1imzkfz</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>CAT EYESSSSS</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imzkfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1imzthu</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>PLEASE help me find nail polish that will match my nail bed colour 🥹</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imzthu</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1in1y1o</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Important steps</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in1y1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1in1q89</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>So shifty!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pda9rn1k7jie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1in19e3</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>❤️🤍Hearts🤍❤️</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in19e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1in1706</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Minimalist VDay mani 🖤</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in1706</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1in0yro</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Press on designs ✨️ 2nd time lucky 🤞🏻</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibr7p39ofiie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1in0nvz</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>I haven’t used press ons since 2008, I’m surprised at the improvement</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in0nvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1in0mwm</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Got got yall - be careful on the swap sub</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1in0mwm/got_got_yall_be_careful_on_the_swap_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1in0br4</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>valentines day nails 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojcgwakxwiie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1imzss6</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>How long do you use a buffer before you change it?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imzss6/how_long_do_you_use_a_buffer_before_you_change_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1imzsj9</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Date night nails</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5px3b9zmsiie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1imzhhh</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Struggling with OPI</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imzhhh/struggling_with_opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1imz41g</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Need to long nails for an event</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imz41g/need_to_long_nails_for_an_event/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1imyrn2</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Help! My nails never dry in the humidity</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1imyrn2/help_my_nails_never_dry_in_the_humidity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1imuteo</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>This colour fills my soul!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imuteo</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1imumll</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Black and white from a newly obsessed lacquerista - kind critique welcome!</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xa0ha4gf8hie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1in540l</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>My nails Valentine day🥰</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lweqw6qewjie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1inkpps</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Cat collar nails</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inkpps</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1ink9l2</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Really proud of my lollipop</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ink9l2</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1injvnf</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>New to nail art and really love the (impressionist?) lavender i painted 🥰</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1injvnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1inj14q</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Update: First hand done 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inj14q</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1initsi</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Magnetos?</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1initsi/magnetos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1inippb</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Cat eyes</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inippb</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1ini6h0</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>DND Sheer Sugar x art stickers 💅🏼</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ini6h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1inhzs7</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>CDG inspired nails ❤️👁️</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inhzs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1inhosa</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Posted late but: year of the snake lunar new year set</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inhosa</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1ingflj</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Cherries nail art</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ju7t724cmie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1infupj</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Life is like a box of chocolates... sorta</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1infupj</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1ind94p</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>My Valentine Nails</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/44x4ak8pklie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1incsmr</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>“Coastal Doodles”</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1incsmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1inc48v</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>My nail tech @nails_emmywynn really outdid herself on this set 😍</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7xs192pblie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1inbzci</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Valentine's Milk Bath Nails</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1veny2tkalie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1inbkt7</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Evil eye set</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inbkt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1inbgg0</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>1 down, 9 to go.</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inbgg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1inal56</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>SNOOPY VALENTINES DAY NAILS</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inal56</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1inaiqq</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Started doing nails. Need help with outlining. What nail brushes do yall recommend?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inaiqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1in9xl5</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>First attempt at making press ons (and using gels). Looking for feedback 💜</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in9xl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1in8j6r</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>My favourite press on nail sets 🥹</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in8j6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1in68bt</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Valentine nails</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iugbd83i4kie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1in5wcr</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>My last set 💕</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kucvh9c42kie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1in5mmo</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Simple valentine set</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in5mmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1in4yid</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Gel Nail Art</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iu4mskm7vjie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1in2y02</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Recent sets I’ve made…what do you think?</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in2y02</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1in2xh7</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Valentines Day Set 😍✨</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3g76bklgjie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1in28s2</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Any horror fans?~</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozq2kdpgbjie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1in1gan</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>New:)</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrkngvcl5jie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1in0tlg</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Valentine’s Day is my favorite</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1in0tlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1in0kue</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Anyone ever use real gem chips on nails?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1in0kue/anyone_ever_use_real_gem_chips_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1imzknb</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>My Valentine “junk nails” 💘</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imzknb</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1imyhz9</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Valentines naile i did</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1imyhz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1imwn05</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Valentines set for my sister</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udwjlgkjyhie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1imu9zd</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6n7rslvt3hie1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Feb 13 08:10:58 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_16.xlsx
+++ b/data/collected_data/2025_02_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C716"/>
+  <dimension ref="A1:C916"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12605,6 +12605,3406 @@
         </is>
       </c>
     </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1ioeb5c</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Valentine's set 🥰</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pm9hkxa6vie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1ioe2zl</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Still perfecting this design…</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioe2zl</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1ioe1g8</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Nails that chips away, how to prevent it ? (Remove if it’s not the appropriate sub)</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ioe1g8/nails_that_chips_away_how_to_prevent_it_remove_if/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1iodzs5</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>What to do about cracked nail under acrylic ?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iodzs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1iodqby</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Black for V-day?</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iodqby</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1iodl0n</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Should these have had less gold or more gold or are they more good like this?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jrazi6mwuie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1iocq4e</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>is there any way to cover this up?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mo70cqswluie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1iocl7y</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Airplane nails?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iocl7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1iocfis</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Kuromi nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iocfis</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1iobupf</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>second time doing dip powder~ valentine’s day nails!</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iobupf</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1iobun2</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Just in time for Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fiaxydmwbuie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1iobpjp</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>I’m literally obsessed. I love my nail tech so much.</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlcvgpgeauie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1iob9xw</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Powered gloves wrecking my natural nails, ways to protect them?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iob9xw/powered_gloves_wrecking_my_natural_nails_ways_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1iob5yu</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Love these for Valentines &lt;3</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8zuautm4uie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1iob1i4</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set ❤️hope yall like it. ☺️</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntqlklcc3uie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1ioadjh</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Help a girl out with her nail colour regret and shape identity crisis!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioadjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1ioa5hw</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>My Valentines nails 🌷🌷🌷</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6k4mbejutie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1io9ze3</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>polish freshly removed, longest they’ve been in a while…what color next?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io9ze3</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1io9yr1</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Obsessed!!!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmf5v0fqstie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1io9a48</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Nakie nails right before one broke and made me lose my mind :(</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg8jd22emtie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1io974t</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Where can I find black sticker nails?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1io974t/where_can_i_find_black_sticker_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1io8bsu</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Ways to strengthen your nails?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1io8bsu/ways_to_strengthen_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1io92pe</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>opinions? tried valentine’s day nails! 💌</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxuex8zgktie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1io8x23</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Set</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vg2empyitie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1io7xvd</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Which brand of press ons has the most narrow sizing? I have super super narrow/small nails. Glamnetic and some other brands literally doesn’t have that info listed anywhere :(</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io7xvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1io7qiw</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Nakie nail appreciation</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io7qiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1io7kys</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>how to do cat eye??</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cjcuyjy6tie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1io7eqg</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Black history month nails my GF did</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uiqib0bf5tie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1io75ze</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Stole the idea and love it</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7tonttbb3tie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1io6nwk</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Valentine set ❤️</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wff4kh90zsie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1io6ocu</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>This was my first attempt at adding details</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6o8pqw3zsie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1io6bcp</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Black Ice</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io6bcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1io69n9</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Painting a Clefairy Nail Set!</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upqrxg3ovsie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1io5wam</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Previous set of French tips of my toes 🥰🥰💘</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0bjayzjssie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1io5uhl</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Pink valentines nails 🩷</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io5uhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1io5g5y</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>How to use nail sticker stencils on curvy nails</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1io5g5y/how_to_use_nail_sticker_stencils_on_curvy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1io4y0h</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Oval or stiletto?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scus070sksie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1io4dee</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Are they fine for Valentine's?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4hrwgq7gsie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1io49tu</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Loving red at the moment ❤️</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io49tu</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1io497f</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jdhkclrbfsie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1io41lp</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Rodeo nails on my natural nails!</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io41lp</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1io3t2c</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Did I pay too much for my nails?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4o9uq3xbsie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1io2c7j</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>DIY Valentines Day Manicure</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io2c7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1io330n</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>The most underrated nail strengthening method!!!</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1io330n/the_most_underrated_nail_strengthening_method/</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1io301r</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>King Heartless Nail Art!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io301r</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1io2yyz</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>OUCH</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7f83yll5sie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1io2vsh</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>trouble pricing nail art</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io2vsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1io2py5</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Solution to stop biting my nails</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0as0utn3sie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1io2gbu</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>My girl did such a great job. Yes, she hand painted that rose 😭</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfct1x5o1sie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1io29gf</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Press on advice</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1io29gf/press_on_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1io1mew</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>How to remove glue from underside of press ons?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1io1mew/how_to_remove_glue_from_underside_of_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1io1gf2</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Favorite Gel X Tip Brand?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g42ywfw8urie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1io1g77</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Neptunium vibe 💙🔱</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io1g77</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1io1977</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>More vday nails....</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io1977</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1io18q0</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Obsessed with press on nails</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io18q0</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1io0zsy</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Red tips for Valentine’s Day ❤️</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpfb8zdrqrie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1io0tj4</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Did my amazing grandma’s nails&lt;3</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io0tj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1io0ljc</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Anime nails?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1io0ljc/anime_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1io0iu5</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Extra nails?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1io0iu5/extra_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1io0ehr</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>First try with water marbling</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqe28flcmrie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1io08cx</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Male at the salon</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4bigc44lrie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1io011u</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Went elegant this time</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5si4l8lnjrie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1inymb0</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Help/Advice</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inymb0/helpadvice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1inyw1l</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Matte cat eye</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inyw1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1inyqd0</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Mooncat polish is the BEST</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhqjmbdbarie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1inypbh</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Do these look bad?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/as0ahfw4arie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1iny7pk</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Made my own jelly nail polish :)</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtbwnbxm6rie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1inyaf3</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Add new color at home a few weeks after having nails done?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inyaf3/add_new_color_at_home_a_few_weeks_after_having/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1iny75t</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Suggestions for nail shape for someone with different shaped beds and types a lot</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iny75t/suggestions_for_nail_shape_for_someone_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1iny22f</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Really proud of these!!</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fckzf4i5rie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1inxwey</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/an238yid4rie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1inwxue</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Any other baby nail techs just itching to do more nails</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inwxue/any_other_baby_nail_techs_just_itching_to_do_more/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1inxlav</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Valentine Nails 💕</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inxlav</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1inxi6q</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Uv/led vagy led lámpa</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inxi6q/uvled_vagy_led_lámpa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1inxanw</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>valentines nails :) ✨</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inxanw</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1inx21t</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>valentine's day set!</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgs3022gyqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1inx0v6</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Matchy matchy 🤷🏼‍♀️ nude valentines 💘💘</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q169o2m7yqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1inwtve</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Heat sensitive colour changing nails!!</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inwtve</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1inwnaq</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>My nail artist lowkey ate 🤭 fav set so far!!</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inwnaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1inwaws</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Pretty in pink</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bm6r6k20tqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1invyqx</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>twin peaks nails + inspo</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1invyqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1invyhr</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Valentine’s set💜♥️</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oat52hhiqqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1invuen</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Glazed donut 🤍</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1invuen</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1inv8us</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>something different</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/axubndghlqie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1inv7oa</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Is this just sloppy or should I expect this with growth? Give her another chance or find someone else?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inv7oa</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1invnvz</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>I am so obsessed</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yf7f19qhoqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1invnex</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>New nails.Giiiiirrllss I'm fell in love</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os2fs8peoqie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1invm4k</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>just got my nails done 💖</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1invm4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1invlwh</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Freestyle valentines set by me✨</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wz30sa4oqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1invg26</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>First Builder Gel Set. Suggestions for Wedding Nails?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2902jkxxmqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1invfq4</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Birthday nails ✔️</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0dbb82wmqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1invf8j</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>First time making my own press ons. Any pointers?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emcst4nsmqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1inv8dc</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Happy valentines day 💓</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gouje8wdlqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1inv6r9</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Help! What nail shape should I go with?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inv6r9</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1inpg3e</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Will topcoat/builder gel help weak press ons?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vl11k5v1apie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1inuzcy</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inuzcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1inqp4c</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Can you glue press-ons to a layer of dip powder?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inqp4c/can_you_glue_pressons_to_a_layer_of_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1inuvqj</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Nude every time!</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inuvqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1inrkol</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Need help to fake a pro manicure</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1inrkol/need_help_to_fake_a_pro_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1inundw</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>I’ve never had Valentine’s Day nails before and I think I’m in love!😍 Also a colored tip?! I’m doing this much more often!</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzgdhlz3hqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1iodppt</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>I'm a happily married woman but I will also happily wear black on Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iodppt</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1iocla3</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Collection organized! 🥰</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iocla3</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1iobhzw</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Don't mind me, just mod podging over my problems 🙃</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iobhzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1iobe3i</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>I want to share my LNY nails since it's the last day!(Lantern fesitival)</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/as2rce6n6uie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1iobdjs</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Vitamin E oil benefits?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iobdjs/vitamin_e_oil_benefits/</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1iob8in</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>❤️Simple Valentines Mani❤️</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iob8in</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1ioaxyw</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Crème nail polish advice wanted</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioaxyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1ioawr3</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Does anyone own Atomic’s radioactive collection?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ioawr3/does_anyone_own_atomics_radioactive_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1ioatrv</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Lemming Lacquer..</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ioatrv/lemming_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1io9hgj</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Beautometry.com Coupon Codes?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io9hgj/beautometrycom_coupon_codes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1io9exb</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>The cost of quality</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbjp56dnntie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1io9bwp</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>My take on a Valentine’s Day mani</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io9bwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1io99eu</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Press on advice</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8u3yss7mtie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1io90zs</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>ILNP Love Story for Galentine's</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io90zs</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1io8pk5</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io8pk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1io8o22</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Clionadh Haul</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io8o22</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1io8mxk</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Looking for guidance</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io8mxk/looking_for_guidance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1io8iy7</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>never enough teal!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io8iy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1io8ind</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Poison for Valentine’s Day 🔪❤️‍🩹</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io8gfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1io8ezf</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Is this a fake?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8he07idetie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1io85mh</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>DIY gold leaf top coat?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io85mh/diy_gold_leaf_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1io7use</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Earthy Zoya Skittle</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97fyudmd9tie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1io7uku</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Essie to the rescue UV gel repair... as a basecoat?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io7uku/essie_to_the_rescue_uv_gel_repair_as_a_basecoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1io7eez</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Regular polish with gel?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io7eez/regular_polish_with_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1io702l</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Valentines Day Mani</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb850jiw1tie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1io5lms</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Valentines (again)</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io5lms</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1io5jev</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>How Much Polish Can Fade</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io5jev/how_much_polish_can_fade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1io56dl</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>What’s everyone’s fave Cirque colors?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io56dl/whats_everyones_fave_cirque_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1io4rrg</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Possible dupe for Earth Angel by Lights Laquer</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68zi2lmdjsie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1io3vg7</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>nail lifting with opi or sally hansen products?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io3vg7/nail_lifting_with_opi_or_sally_hansen_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1io3slf</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>In your opinion, what indie brands are producing the best or most creative jellies or crellies?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io3slf/in_your_opinion_what_indie_brands_are_producing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1io3oc1</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Dupes: Clionadh "Plateus" &amp; WUB "Feature Creature"</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdpeow4wasie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1io39i2</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Showing love to some underused thermals 💕</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io39i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1io31wm</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Valentine’s Day mani!!!</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io31wm</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1io2v4a</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Recommendations for clear polish?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io2v4a/recommendations_for_clear_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1io24qw</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Decided to see what would happen if I mixed the two prettiest colors I own</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io24qw</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1io2199</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Opposite polarity magnets</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1io2199/opposite_polarity_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1io15pl</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>New Clionadh brushes?! 😍</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv6dnmlzrrie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1io0nm7</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Help, I need advice 😅</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io0nm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1io093v</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>indie brands from etsy, part 2: Daisy Chain Polish</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io093v</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1io04fr</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Not sure what to do about this</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xci54c8dkrie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1inzvtl</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Your Heart’s a Black Hole</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oyppp0alirie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1inzd8l</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>My Cirque Colors Lucky Bag</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inzd8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1inz5er</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>The more I look, the more I love her</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qphp23w9drie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1inyu1g</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Subtle Valentines manicure</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inyu1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1inyqp2</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Abracadabra abra-ca-daaaaabra 🪄 feel the beat under your feet the floor’s on fire 🔥</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inyqp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1inypco</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Mooncat Mercury's tears</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1inypco/mooncat_mercurys_tears/</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1inyovy</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - Sunken Treasure</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tplokjj1arie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1inym0d</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Valentines nail art 🩷</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inym0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1inyg3w</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Post holiday in Morocco manicure</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inyg3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1inyfme</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>ILNP Get Cozy vs Mooncat What is my Purpose</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g72fa7n68rie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1inxkwv</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Valentine’s week mani</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inxkwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1inxj7a</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Look -A-Likes?</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcty62xq1rie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1inxhlj</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Update: the heart magnetic polish hack works (sometimes)</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11ubincf1rie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1inxea2</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Tink’s Wings🦋🩵💖</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cbodwpxp0rie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1inxd82</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Hearts without the paperclip 🩷</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5umwj68k0rie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1inxbpu</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>As The World Falls Down 💫</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inxbpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1inopn8</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Valentine's day 💘</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8ami9oh1pie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1inq6aq</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Looking at my nails in the library instead of working on my thesis</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43yrwaefhpie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1inx303</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Anti-valentine 💔</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8q27vjhmyqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1invz1w</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>There’s your problem. Someone set your brush to summer.</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w6y66aqmqqie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1invb1h</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Water Marble for my Birthday! 💜✨</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1invb1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1inutyh</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Layering Jellies and Magnetics</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inutyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1inulmw</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>My best pink!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inulmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1inuemy</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Some Simple Hearts</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1tcrg0cfqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1inu3v8</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Fox in the Spring Court dupe???</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1inu3v8/fox_in_the_spring_court_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1intyce</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>I'm obsessed</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1intyce</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1intm6q</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Magnetic hearts Valentines ❤️</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ggl4xy5k9qie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1int463</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Pink? For Valentine’s Day? Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grzbdqas5qie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1insw9q</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Tink’s Wings🦋🩵💖</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1insw9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1insb22</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Valentine's nails!!!</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1insb22</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1inry2s</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>🐧✨️Penguins ✨️🐧</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inry2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1inrs62</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Valentine's Day Nails 💋❤️</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inrs62</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1inrdth</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>V-day look.</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wo5io7a5spie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1inowsx</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Placed my first "Fancy Polish" Order!! Started with 57 polishes in my cart, these are the final 6 that made the cut!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ljsgcwi3pie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1inj5fb</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Looking for red-leaning orange polishes with specialty finishes</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inj5fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1inngij</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>I was inspired by everyone’s V Day nails ♥️🩷</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3f73wrjjoie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1inn0no</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>ARCANE / JINX Nail Art | Hand-painted by me | Let me know what you think!</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sha60108tt5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1iocz60</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Be my valentine hoe!</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqo6se2zouie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1ioabt7</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>nail gift</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioabt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1io7x0i</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>The first ever junk set I done and it a flop mostly cuz of application and way too much top coat, should I redo it now cuz I really like the vibe of it? Idk what do you think</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io7x0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1io7p7r</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Lace stilettos and chrome ♥️ tried a new technique!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tudt4ukz7tie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1io7one</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Valentine's Day Nails</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4r7h3tu7tie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1io68m1</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Painting a Clefairy Nail Set!</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2c2dw5cfvsie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1io5hkh</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>polygel nails set</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1io5hkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1io4zlw</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Some nails I made based on some of my favorite classical piece of music. Guess what the inspiration was!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acgw7cb5lsie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1io3ebg</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqjpr0qs8sie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1io1m80</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Valentine's nails🥰🩷</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2f1m620hvrie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1inyd4j</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>All of my nail practices so far 👀 what do we think ?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inyd4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1iny3fs</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Really proud of these!!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9t3v1czr5rie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1inw6kx</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Moodboard inspo ✨🍒</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inw6kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1inunao</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Nail art with small dried encapsulated flowers</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkdum7b3hqie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1inttul</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inttul</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1int8eh</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>My first press-on set</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zndibdmn6qie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1insooi</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>wedding florals with a cultural nod 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1insooi</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1insf7y</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>We’re having a brat girl Valentine’s this year 💚</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfbl1x7i0qie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ins37e</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Labradorite Nails</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2ha93wgrxpie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1inr6aw</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Temu supplies?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1inr6aw/temu_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1inqhps</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Who more lover of black</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzep5pf8kpie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1inoaz5</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Bday to Vday nails</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1inoaz5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Feb 14 08:10:39 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_16.xlsx
+++ b/data/collected_data/2025_02_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C916"/>
+  <dimension ref="A1:C1114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16005,6 +16005,3372 @@
         </is>
       </c>
     </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ip5nuk</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>My V-Day gift to myself.</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip5nuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ip5nsx</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Valentines nails 🎀</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egfbcy2e92je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ip0vw3</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>In desperate need of help</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip0vw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ip3wm5</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Weird toenail growth - help</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip3wm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ip4h8k</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Nail polish / products for hands with eczema?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ip4h8k/nail_polish_products_for_hands_with_eczema/</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ip5351</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>My Valentines Day nails (diy)</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t5mi4kfs12je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ip41w4</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>I’m a beginner so don’t judge too hard! What do you think of these? I jazzed up the photos a little hehe ☺️</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip41w4</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ip3n5j</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>My Valentine Nails 💅💅💅</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4npg73ek1je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ip3fxa</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>The Palette Cleanse - Funny Bunny + Bubble Bath</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip3fxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ip3fsk</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Alternative to gel/acrylic</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip3fsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ip3b6t</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Natural nail growth ❤️</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip3b6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ip2vm7</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Newbie Needing Some Sparkle!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ip2vm7/newbie_needing_some_sparkle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ip2s9a</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Why does my nail grow like this</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sugzhnn9b1je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ip2j9e</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Can I fix this janky nail</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lizy7qj81je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ip2ggy</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Cutesy press-on nails 🎀</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip2ggy</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ip2fln</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Anyone have a cheap cream gel dupe?</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ip2fln/anyone_have_a_cheap_cream_gel_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ip27jh</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>I am not sure what to do</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip27jh</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ip2bux</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>2nd Set Ever</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lndk4ji61je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ip229n</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>I figured, hey I love getting sweet treats on Valentine's Day, so why not?</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9qibpjs31je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1ip1pmo</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Didn't plan on doing Valentines nails yet here we are</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip1pmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1ip0x62</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>DIY Jelly Valentine's lewk! With chipped/broken improv.</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip0x62</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ip0vmi</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Advice needed: fix or refund?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip0vmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ip0h9f</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>My Little Local Spot Appreciation Post</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip0h9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1iozyzr</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Got this idea from Amazon press on art</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xldgqxmj0je1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1iozup1</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Canadian gel polish</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iozup1/canadian_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1iozu6z</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Here are some cute designs that I did🥰 what do you like more?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iozu6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1iozok0</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Acrylic Nails for Guitarists?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iozok0/acrylic_nails_for_guitarists/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1iozlsz</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Conventional nail polish over gel with soak-off base coat makes it come off</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iozlsz/conventional_nail_polish_over_gel_with_soakoff/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1iozhkm</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Subtle heart for valentines</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xs5eqey1f0je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1iozdv8</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Simple valentines design</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iozdv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ioywgw</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>how do i make these nails more appealing</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vcl1t3k90je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ioz7an</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Valentine's Day press-ons 🩷🩷🩷</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfdx95xcc0je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1ioz659</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>I Love my nails red♥️</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6oz1u1b2c0je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1ioyjgk</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>my first set with extensions in idk how long</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioyjgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1ioxjeo</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Shape change, regretting it already lol I've always had square nails so I'm good at square, I can't get these almonds? to look good 😭</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jp959q4xzie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1ioy697</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails. How did I do?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sm0wgugt20je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1ioy1ze</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>After 30+ years of chewing my nails i finally stopped and started loving them instead &lt;3</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioy1ze</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1ioxy96</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Last minute nails</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/feks8sxx00je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1ioxlg7</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>New set to match the flash of my labradorite ring</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioxlg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1ioxdmi</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Carebear themed nails</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8zj30dxvzie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1iowacx</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Xmas/Vday nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jijp5obmmzie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1iovln1</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Acrylics on broken nail bed.</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iovln1/acrylics_on_broken_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1iovb1e</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>How do you maintain your “cuticles”?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iovb1e/how_do_you_maintain_your_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1iovd9p</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Can you do an acrylic overlay on natural nails and glue press ons</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iovd9p/can_you_do_an_acrylic_overlay_on_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1iovald</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>First time doing gel myself, also tip for mixing gel colors??</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iovald</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1iov1bp</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Camo marble?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo5y13btczie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ioune5</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Need help understanding nail extensions &amp; application methods</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ioune5/need_help_understanding_nail_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ioulin</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>What I asked for vs What I got. 💅🏻</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioulin</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ioupga</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Self care day</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4wj9u89azie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ioun4j</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Help finding neutral color to match my natural nails</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4kw27pq9zie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1iouie7</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>First time cat eye 🩷</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m49u1xro8zie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1iougzv</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Pink chrome and magnetic heart ❤️</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iougzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ioug0t</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>new press-ons</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioug0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1iou4er</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>just a nail tatto 🤩🌹</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29u15jzn5zie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1iou1r5</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Thick edges on French tip</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iou1r5</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1iotru6</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>My DIY Valentine Gel Nails on my natural nails</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iotru6</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1iotqqz</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Since it’s Valentines Day Eve, I wanted to share my gel-x set</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iotqqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1iotkvb</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Care Bear nails!</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iotkvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1iot5et</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>First set of character art!</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iot5et</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1iota8g</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Does eyeshadow on gel nails actually work?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iota8g/does_eyeshadow_on_gel_nails_actually_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1iotb5y</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Christmas nails I did ❤️</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o017v3zfzyie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1iot4dp</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Chrome with some cute little hearts for Valentines Day</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2dsgayzxyie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1iosumn</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Hey y’all, I’ve recently been getting into doing my own nails! This is my valentines set but I have a question!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5029h26wvyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1iosedu</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Why do my nails grow sloped and outwards?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iosedu</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1iosdzz</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>What is your next set?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iosdzz/what_is_your_next_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ios8ri</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Simple valentines nails *muah*</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxekkqy7ryie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1iori60</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Valentine's nails today by yours truly 🥰💅</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2rz2rynlyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1iore4k</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwnucagukyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1iordw1</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>I want to start getting my nails done</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iordw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1ior9p5</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Pastel party on my nails</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev4q5hlxjyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ior54s</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>My new nails</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu4y1xkziyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1ior3p9</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Recap Barbie sets - S01</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ior3p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1ior2xb</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Cow nails 🐄</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ziknysiiyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ioqzv8</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Vday nails this year ❤️</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3f158evhyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ioqkte</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Chocolate nails</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dybcqz3teyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ioq8yu</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Valentine Nails by Me!</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioq8yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ioq6d2</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Pink V Day Gel Nails</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioq6d2</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ioq4s1</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>matching tips &amp; toes 💅</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p97o0xtfbyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1iopw0n</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>My first set ever</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txnkyojl9yie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1iopw0f</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Cutesy Valentine’s flowers I tried doing</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iopw0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1ioprqu</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>dreamy valentine’s nails ☁️💕</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioprqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1iopqaq</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Cat eye pink! Can you tell which have tips?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iopqaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ioph2e</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Nail art done on my natural nails</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yv90f4h6yie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1iook48</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Before and after applying press on nails</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iook48/before_and_after_applying_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ioo857</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Is this possible?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ioo857/is_this_possible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ionvyg</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Valentines 💝 day mani</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ionvyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ionpug</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>February shorties</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/php2o0setxie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1iongq5</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>before and after</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iongq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1ionax2</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Did a Valentines set 💕</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ionax2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1ion80c</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>New set on myself ♥️👹</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ion80c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1iohp7n</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>I got a touch of onycholysis from my last nail job. Dirt stuck under nail bed</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/huckvxq8ewie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1iomx0f</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>I did these nails for my wife and daughter for valentines day! It's my first time doing nails how did I do?</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iomx0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1iogf8s</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Need advice</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iogf8s/need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1iom2wb</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Everyone thinks I have Barbie nails, but that's not what I wanted 😭 B is the first letter of my boyfriends name</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uo4zrhm5hxie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1iohb6i</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iohb6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1iofx4c</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails with a twist 🐝🫀</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iofx4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1iomf53</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>I guess this is my kind of valentine's nails</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9dqsppqjxie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1iomb2w</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Manicure for vacation😜</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnibpyjsixie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1iolyx8</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Love them ❤️</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1oh9saagxie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1iolxss</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>I'm just a girl in love with thin french almond nails! Old set, but should this happen again?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdsvs31xfxie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1ip5qbm</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Bluey Valentine’s Day💌🥰</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip5qbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1ip5eeb</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>What's up with my free edge?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c73mxkns52je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1ip4k21</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>I thought painting my dominant hand was hard</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gv2xth7v1je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1ip476e</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Vday nails/first post</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5abnpovq1je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1ip3tkz</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Holo Taco Lavender Syrup</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hqkkybem1je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1ip2p5g</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Cherry nails for V day 🍒</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb3qhhxba1je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1ip1x2w</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Gel polish removal</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ip1x2w/gel_polish_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1ip1qcy</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>ISO cool toned pink and purple polishes?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ip1qcy/iso_cool_toned_pink_and_purple_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1ip1g02</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>it’s a holo partyyy 🥳</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1hx55pzmx0je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1ip1f9v</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>💅💖🎀✨</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip1f9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1ip14ox</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Showing off simply done Valentine nails!!</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip14ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1ip14nn</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>🎀🩷</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6nbaxvlu0je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1ip13xr</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Wearing a color I know my husband will love for Valentine’s Day! ❤️</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o71ax2ceu0je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1ip0zil</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Cirque Lucky Bag came just in time for my Valentines Day mani!</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wkv31v8t0je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1ip0t2q</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Found my nail stash</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xso57idir0je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1ip095y</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Pink, pink, and pink-ish for Valentine's 💕</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip095y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1ip0601</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Mardi Gras Nails! Take 2. 🎭🎊</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip0601</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1iozsq3</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>another dollar store win from la colors 😻</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5icer80i0je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1ioze6c</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>💝 Valentines/Chinese New Year 🐍</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxjgnl75e0je1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1ioz04o</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>My obligatory Valentine's mani</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihsosfwha0je1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1ioypg4</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>gel allergies and press ons</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ioypg4/gel_allergies_and_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1ioyjo5</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>very pink vday manicure :)</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t722dbp960je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1ioyilx</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Vortex Shaker?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://a.co/d/46eC1UX</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1ioyid6</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>How to sell my polishes?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ioyid6/how_to_sell_my_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1ioyga8</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Favorite sheer polishes ? !</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioyga8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1iowub5</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Fly 25 feat. my fave plants !</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iowub5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1iownuk</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Got my mini haul in the mail today but unhappy with one of my purchases: ILNP’s CEO is more patchy than expected.</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iownuk/got_my_mini_haul_in_the_mail_today_but_unhappy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1iowgqz</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Pour one out 😭</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nix5yfp5ozie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1iowesb</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2b9tenknzie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1iowc3n</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iowc3n/emily_de_molly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1iovwna</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>A quick velvet Clionadh skittle to compare their psychedelic selections</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jty13elmjzie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1iovndt</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Pink!</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnc2jinkhzie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1iovjrg</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>wicked ivy ✨</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iovjrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1iovhsa</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>❤️V-Day Mani❤️</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iovhsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1iov34l</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails- Scum and Villainy</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iov34l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1iouvlm</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Couldn’t decide red or pink, so I did both</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9956eb6kbzie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1iouq4c</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Perfect intersection of joy</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iouq4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1ioumky</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Mani</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tz5px60m9zie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1ioubdk</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Red for Valentine's? How original</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioubdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1iotgim</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Swampy Sweethearts 💚</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iotgim</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1iot3bx</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>my vday pick - fields of lavender</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iot3bx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1iot3ax</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>anyone know of a nail polish/es that could be used to recreate this look?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtsw4sgrxyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1iorde8</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Nail Envy Caused Insta-Yellowing?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iorde8/nail_envy_caused_instayellowing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1iot0l7</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Too similar (?) 🥲</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iot0l7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1iosukn</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day Laqueristas!!!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iosukn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1iospi2</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of I-Scream’s House Of Horrors!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iospi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ioshkk</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Nobelium for Vday</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioshkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1iosbev</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Some Poison for Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r31o8l3sryie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ios5gm</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>After two decades, I stopped biting my nails! 💅🏻 (Sally Hansen, Hyp-nautical)</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v81ymtfiqyie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1iorqff</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Octopuses have three hearts, so I’m counting this as a Valentine’s Day Mani</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iorqff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1iorodz</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Working in sub zero temperatures turning my nail polish orange? 🍊</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iorodz/working_in_sub_zero_temperatures_turning_my_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1iorga6</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Lucked Out with Some Free OPIs</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnks1naalyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1iopdma</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Looking for a color like this</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtwpqhnr5yie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1iopm1y</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>A little evil for V-day</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iopm1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1iopbvq</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>What polish is this? Anything similar?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwkl3rwd5yie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1iopbqc</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Am I a freak of nature?! (Thermal polish issue)</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iopbqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1iop5l4</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Hearts 💕 (and all of my other thermals)</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iop5l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ioooyj</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>💖 Valentine’s Day mani! 💖</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioooyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1iookym</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>I found the secret to a long lasting mani…</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iookym</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ion1mu</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Valentines idea I’ve had a while</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ion1mu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1iomg1z</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>❤️⛓️Chains &amp; Whips Excite Me⛓️❤️</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iomg1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1iokmg1</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Wearing two different brands' cat themed Valentine polishes</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42vlfq5n5xie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1iojfz8</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>This glitter 😍</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iojfz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1ioji7n</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>HT DavidsTeal vs MC Abandoned Boardwalks?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ioji7n/ht_davidsteal_vs_mc_abandoned_boardwalks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1ioieg7</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Your Heart's a Black Hole, Psycho</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g3fg42ujlwie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1iohfka</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Anyone tried Cracked's jelly formula?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iohfka/anyone_tried_crackeds_jelly_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1iogkha</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Business in the front, party in the flash</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iogkha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1iog8i7</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>You already know it's Valentine's</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuqk2jhkwvie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1iofgtc</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>ok i’m a metallic girlie 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iofgtc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1ioepby</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>I thought this sub could relate 🙃</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8jye2cobvie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1ip5hze</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Sorta valentines nails.</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq1nsn5772je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1ip5gj4</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Happy Valentine's Day💕</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip5gj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1ip44yp</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Hoppy Valentines Day 🐸 💕 (credit: Alex @ Camellia Nail Bar)</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip44yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1ip3k5r</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Valentine's Day 💘 (not experienced)</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip3k5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1ip2rpc</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>🎶I can paint myself flowers🎶</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip2rpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ip2nq4</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Valentines nails ❤️ (hand painted by me but not my original designs ) was very proud of the middle finger!</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1dan76w91je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1ip2lre</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Stained glass again… but Valentine’s Day edition!</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip2lre</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1ip20v3</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Wanted something a little different for V Day</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncvwo1ie31je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1ioxegm</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Nailart of this week (inspi given by my 4 YO daughter : pink/flowers/sparkles) 🌸</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4a4n9zm4wzie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1ioudlu</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>I'm so proud of this set!</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioudlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1iotixo</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Just did my nails!💖</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/up4l16u11zie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1iot628</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>My Valentines Day Set 😊😊</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm23ibxcyyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1iot1tk</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Matching valentines mani with my mini 💕</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5n41s4mfxyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1ioslaa</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Valentine's Day Nails</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioslaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ioshdf</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>What do you think? Some correction</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioshdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1iorlp2</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Recap Barbie sets - S01</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iorlp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1iorcem</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Valentines nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0wo4vphkyie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1ioqhhc</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Some of the Vday nails my Wife has done this week!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioqhhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1iopexz</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Uhh I might have overdone the hearts this year 💕</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iopexz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1iooiir</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>new set! absolutely in love</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iooiir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1iomyeu</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Vday nails</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iomyeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1ioml7e</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Baby Blues for Valentines 🩵</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioml7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1iom3m5</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>some custom press ons i did ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iom3m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1ioliz0</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Strawberries and cream valentines</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ioliz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1iol5ry</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>My clients are getting March Ready ✨💚</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iol5ry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1iojxpl</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>I did y2k valentines nails</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iojxpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1iohp9s</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Rare? A very particular set</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i02wsyc9ewie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ioenro</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Valentine's Day nail art I did 😊🩷</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hljpwgd2bvie1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Feb 15 08:09:20 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_16.xlsx
+++ b/data/collected_data/2025_02_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1114"/>
+  <dimension ref="A1:C1324"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19371,6 +19371,3576 @@
         </is>
       </c>
     </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1ipwsw8</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>My Valentine’s Nails</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6e1yiq8g9je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1ipwi0y</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Ocean mood🪼🐬🐳🐠🩵</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gxvnyn4c9je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ipwgb3</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Rate my nails</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijq583ugb9je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ipwevk</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Hey friends, which nail shape suits me best? 1 or 2? Thanks for your help 💙💚</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipwevk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ipw2pn</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Did i go too short this time?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipw2pn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1ipvx78</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Did i go too short this time?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipvx78</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1ipvt65</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>VDay glue ons 💕🍒🎀😍</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipvt65</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1ipvs1d</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Getting used to typing again</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipvs1d/getting_used_to_typing_again/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ipvpbp</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Treated myself, regretsss 😤😤</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipvpbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ipuycn</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Fresh nails and I’m obsessed with them!!🤩</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipuycn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ipuv5w</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>press on nail glue residue</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipuv5w/press_on_nail_glue_residue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ipusg0</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Nail Glue Dilemma</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipusg0/nail_glue_dilemma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1iptayr</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Bubbles</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iptayr/bubbles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ipuiel</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Birthday nails💜🗡️</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipuiel</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ipu2ij</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>My fave sets I’ve done!</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipu2ij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1iptwk2</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Sleepy pink press ons just in time for Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iptwk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ipss2m</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>WIP of my next Kingdom Hearts nail</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipss2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ipsnfe</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Best gel no-wipe top coat?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipsnfe/best_gel_nowipe_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ips44k</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Happy Valentines nails</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ips44k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1iprx83</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Valentine's Day set</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iprx83</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1iprilo</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>What shape to try next?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iprilo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1iprhaq</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Which shape is the nicest for my hand</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iprhaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1iprckz</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iprckz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ipr4wu</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Tried GelX on Tuesday. I've already lost 4 nails... Help!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipr4wu/tried_gelx_on_tuesday_ive_already_lost_4_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ipr0i7</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Valentine's Nails</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hpi1nthhm7je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1ipqn6r</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>the painting vs the palette</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipqn6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ipqigl</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Help: Elevating My Nails</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qliv0ffjh7je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1ippmxa</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Manicurist using her own nail to remove gel while painting my nails?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ippmxa/manicurist_using_her_own_nail_to_remove_gel_while/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ippx06</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>2 days post-manicure in Queens, NY</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xheljxfwb7je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1ippi1k</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>My Valentines Set ♡</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ippi1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1ipp8kv</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Air dry / no cure vs. UV cured primer</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipp8kv/air_dry_no_cure_vs_uv_cured_primer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1ipomu2</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Who doesn’t love a plaid moment</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipomu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1ipo6tf</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Dip nails w extensions</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rci7vb9aw6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1ipo4un</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>First attempt for french tip nails? Any views?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0w2w18tv6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1ipo3a8</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipo3a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1ipo0im</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>At home hobbyest- tips for nail drills!</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipo0im/at_home_hobbyest_tips_for_nail_drills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1ipo0cj</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>First time using press ons</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipo0cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1ipnv0j</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Gel x nails for valentines that I did on myself. I'm pretty proud of these!</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7ie9zlft6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1ipn6w4</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Please help! 🙈</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1k95ykysn6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ipn51y</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Happy V day, babes 💕</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/np7syqydn6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1ipmysr</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Galentines Set ❤️</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmamhjcyl6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ipmy4b</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>My husband calls them my Guy Fieri nails.</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipmy4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ipmj1z</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails 💖</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipmj1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ipmf2b</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Simple Valentines nails :)</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipmf2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1iplv5p</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>My nails for this valentine ❤️</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ozb1lf9d6je1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1iplnpu</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Cat eye hearts</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rf02y6mhb6je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1iplc80</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>my nail tech really popped awf!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qn8kzbk196je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1ipkwlw</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Happy Valentine's Day! This is my set for today.</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipkwlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ipkj0o</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Absolutely love this set</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipkj0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1ipkdxa</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Which nail shape is best on me?</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipkdxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1ipf536</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Are my nails as bad as I think they are? Inspo pic last photo Femmy nails found on pinterest.</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipf536</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1ipkb90</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Valentines nails! *reposted for better picture*</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y40x421z06je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1ipk7nn</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Voltage!</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipk7nn/voltage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1ipjwtu</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Gel Polish over Regular Base Coat</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipjwtu/gel_polish_over_regular_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1ipk249</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>All handpainted by me, on me.</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzhx4aryy5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1ipjq10</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Cat Eye Nails</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c9fz565fw5je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1ipjps7</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Cat eyeee</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipjps7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1ipjd5h</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Valentines Day Nails</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8p6kd1aqt5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1ipjabm</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>HELP HOW DO I GET MY NAILS BACK TO NORMAL</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipjabm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1ipj53d</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Took Constructive Feedback &amp; Did New Set</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzl89pgyr5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1ipj4bc</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Valentine’s Day 🫶🏽🩷💅🏽🏳️‍⚧️💘</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipj4bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1ipid6l</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Bridal Nails</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sre7r902m5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1ipiyhe</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Valentines nails I did on myself</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhiwatlkq5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1ipien2</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Again, much more subtle than I would usually do, but I'm obsessed</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipien2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1ipidhr</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Valentines mani</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipidhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1iphh3x</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Valentines nails. I think this is the best set I’ve ever done</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iphh3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1iph27v</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>DIY it's also my wedding anniversary today</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iph27v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1iph5ac</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>How to narrow nails?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/la3k4wbyc5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1ipgyn1</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day Look</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yicze1ajb5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ipgssv</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Just finished this set!!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9rs7syaa5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ipggij</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>HVD Nails!</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipggij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1ipg3ih</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails, basic but ol faithful French tips</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1vf1ao255je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1ipg3du</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Atomic Polish - Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipg3du</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1ipfp93</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day! My vday set and maybe favorite set ever :)</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pg10tw9325je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1ipfm94</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Barbie Loving You set - Happy Valentine everyone</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipfm94</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1ipfjcj</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Valentine's Nails ❤️🖤</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27w1jljv05je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1ipfdsd</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me better?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipfdsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1ipfa1h</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipfa1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1ipf5lg</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Finally solved being able to have long nails and typing</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5a2a40v3y4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1ipexon</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Retsuko Nails!</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wlvaed4w4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1iperof</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>6 months of my manicures with nail art &lt;3</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iperof</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1ip6mz9</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Cat scratched my gel nail - how to fix?</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip6mz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1ip7i6w</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>OPI repair mode question</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ip7i6w/opi_repair_mode_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1ipcved</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Help.. nail tech promised no damage…</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipcved</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1ipdc79</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Glass nail file ruining my nails??</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipdc79/glass_nail_file_ruining_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1ipdo6m</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Finally stopping biting my nails</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2fw2mpnm4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1ipe4dg</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Should I ask to have this nail fixed?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipe4dg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1ipe1gd</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>V-Day nails ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qlai3xip4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1ipe11b</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Caping y pincel 🖌️  les gusta??</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38q2e3cfp4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1ipdqxc</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>soap nails🫧 (aka bubble bath  lol)</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8r4km3bn4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1ipdf3n</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>I messed up my brand new nails</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipdf3n/i_messed_up_my_brand_new_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1ipdc4h</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Beginner Valentines art attempt</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du23uk32k4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1ipcy38</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Happy Valentines Day ✨💌</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipcy38</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1ipctrl</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Base???</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipctrl/base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1ipcqy9</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Finally finished this set after 3 days 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipcqy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1ipcprx</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Feeling extra cute in this set 💕🐢</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rjqgzp3f4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1ipclzr</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Looking for help</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18gdb3a9e4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1ipchpx</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Am I the only one?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipchpx/am_i_the_only_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1ipcfx2</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>I could use some recommendations?</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ipcfx2/i_could_use_some_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1ipcfl3</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Happy Lover's Day 💕</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipcfl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1ipvy1f</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Valentine’s skittle 💕</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipvy1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1ipudh2</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>dupe for mooncat’s banquet of breadcrumbs??</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyrmt7ull8je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1ipt75s</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Mani!</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gywa6spl88je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1iprux6</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Question about Lurid Releases</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iprux6/question_about_lurid_releases/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1iprowp</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>KBShimmer released a 30# horseshoe magnet!</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iprowp/kbshimmer_released_a_30_horseshoe_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1ipr35h</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Look ♥️🦋</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipr35h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1ipqurd</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>❤️🖤 Happy Valloween 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/diewimrvk7je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1ipqpoj</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>valentine’s nails :)</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x62wi6rij7je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1ipqayb</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Trying to outdo the sidewalk</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipqayb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1ipq93s</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>China Glaze at Big Lots</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/foajm8h0f7je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1ipq7na</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>I gasped so hard I choked 😅😂</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc7s3mone7je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1ipppl5</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>I normally paint my nails all one color . Decided to try something new and I’m not mad at it. Anyways Happy Valentine’s Day to all of you 🫶🏾🫶🏾🥰</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shljowoz97je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1ipp8n4</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Valentine’s nails theme = burning love</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56rut96m57je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1ipp461</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>New Nails, who dis?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipp461</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1ipoyzj</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day Lacqueristas!</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipoyzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1ipoub5</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Pink for Valentine’s!</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4jbmz8327je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1ipolhq</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Cooties for Valentine's Day 😆</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipolhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1ipnypw</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Best tool for hang nails?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ipnypw/best_tool_for_hang_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1ipnp4h</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Sally Hansen Miracle Gel... How does it stay?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ipnp4h/sally_hansen_miracle_gel_how_does_it_stay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1ipnnq0</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Purps ombre mandalas</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipnnq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1ipncch</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>I can’t believe I almost got rid of this one! Any recommendations for other polish that looks like it’s glowing? 🩷</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipncch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1ipn03i</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails 💘</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipn03i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1ipmubs</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Any Dexter fans?</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5aanfxpxk6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1iplt2g</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>🩷Valentines Day skittle🩷</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iplt2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1iplodo</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Blake flake taco dupe</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onqe9wcqb6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1ipljx0</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Valentines mani 🩷🧡💛</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipljx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1iplhh5</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>another valentines mani :))</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/foo1n8n7a6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1ipl0z5</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>My two simple v-day looks :)💘</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipl0z5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1ipkuf1</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>anti v-day, feeling blue in the best way</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipkuf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1ipkomt</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Psilocin</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/432uo4cx36je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1ipkmp8</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Looking for a nail polish similar to this discontinued OPI - a red with oranges and pinks in it</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/platpzp426je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1ipkmnr</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>photo dump of 🌖🐈‍⬛’s Star Destroyer in every lighting I could think of to try and capture how ethereal it actually is</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipkmnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1ipkj4u</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Th1rt3en - Clionadh (unmagnetized)</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipkj4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1ipkbos</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Happy Valentine's Day 💝</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipkbos</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1ipk6jo</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Sealed with a Kiss</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipk6jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1ipk157</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Matte pink for Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tggwirry5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1ipjq54</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Too early for mini eggs?</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkaa04qfw5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1ipjk6g</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Best quick dry top coat you can buy in store or on Amazon?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ipjk6g/best_quick_dry_top_coat_you_can_buy_in_store_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1ipj3cf</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>It's Galentine's Day, girlies ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipj3cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1ipir3m</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Maelstrom after 2 weeks of wear 🌊</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/014l5ar0p5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1ipicv7</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>First Lurid and it stole the show</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipicv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1ipic74</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Obligatory V-day Nails ❣️</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fy3zpifrl5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1ipi8rw</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Hello all! Is it normal for nail artists to use the same designs as others?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ipi8rw/hello_all_is_it_normal_for_nail_artists_to_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1ipi7sv</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Looking for gift suggestions for someone who is really into nails</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ipi7sv/looking_for_gift_suggestions_for_someone_who_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1ipi2oh</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Thermal on my commute</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipi2oh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1iphoqm</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Clionadh order arrived just in time for Valentine’s day😍</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3o9yua0h5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1iphneq</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Kbshimmer Northern Exposure dupe?</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iphneq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1iphmod</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Releases and sales today</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iphmod/releases_and_sales_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1ipc8kl</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>🤡 Mani for days when you just feel like this</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipc8kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1iphlk7</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>ILNP Sidekick vs MC Shattered Glass?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iphlk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1iphcwj</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day💕</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iphcwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1iphb0r</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Wildflower Mind Your Own Biscuits and Life Will Be Gravy</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7w16b45e5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1iph7yo</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>When your v-day mani is red and white because your hands are both dry and cracked/bleeding 😌</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iph7yo/when_your_vday_mani_is_red_and_white_because_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1ipgvat</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>A classic for Valentine’s Day ❤️🍷</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipgvat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1ipgr9a</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Help my (fake) nails keep falling off</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipgr9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1ipgqu8</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Maryann by Zoya on natural nails</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipgqu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1ipglpd</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>✨One can never have too many galaxy colored polishes 🌌 ✨</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7lmw2a0v85je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1ipghlc</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Pink for Valentine’s Day? Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipghlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1ipggvm</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Vday Pt 2 Bugaloo</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipggvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1ipg9uj</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Valentines Vanessa Molina</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipg9uj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1ipg935</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Polish Me Silly "Barbee on the Glow" vs. MC "Merkitten"</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipg935</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1ipg3xt</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Successfully frankened ILNP Lightwave</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oqjrabsw45je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1ipg408</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Atomic Polish - Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipg408</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1ipg2cj</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Mooncat Foxfire vs INLP Imagine That</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ipg2cj/mooncat_foxfire_vs_inlp_imagine_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1ipfs0q</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>(gifted) Arcana Lacquer’s “Beyond the Myth” collection is available today at 6pm EST! Website is open for wish-listing ✨</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkqoyfdo25je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1ipfqjh</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>My cat is unimpressed by Lavender Fields</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3lpg7kjc25je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1ipflsn</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Anti-Valentine’s Day Mani</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipflsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1ipfies</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Vday skittle ❤️🩷</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipfies</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1ipfgl6</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Perfect Love</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipfgl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1ipfewg</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Creative (Cheap) Alternative to Plastic Swatching Objects</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fke28ogyz4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1ipf985</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>The better black polish</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ipf985/the_better_black_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1ipf1hk</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Valentine's Day Nails</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipf1hk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1ipeplx</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>A Valentine's Jelly Gradient!</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0m1naxju4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1ipekd0</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Why it’s dangerous to leave your house</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4atrd5hit4je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1ipdkt7</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Valentines Layering Experiment</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipdkt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ipd5hr</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Valentine Skittle</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipd5hr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ipd1vc</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Preventing staining</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ipd1vc/preventing_staining/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1ipcj7r</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Magnetic for Valentine's</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/121ffcnld4je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1ipcezm</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Rose Nails 🌹</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipcezm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1ipcefu</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>I am so underwhelmed by the new Mooncat collection</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ipcefu/i_am_so_underwhelmed_by_the_new_mooncat_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1ipc9xo</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>My first magnetic with matching(ish) earrings for Valentine's</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipc9xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1ipc5ok</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>💛💜Chalky Hearts🩷💚</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipc5ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1ipbu2r</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer Valentine’s Day Skittle</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipbu2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1ip8jie</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Herzlack nailpolish experience</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ip8jie/herzlack_nailpolish_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1ip75vm</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>I DUPED FLAMINGLOW 😱</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip75vm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1ip72hm</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>My first easy valentine mani</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2fbtp5as2je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1ip04o1</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>I’m a Brown mood</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svyb8ym4l0je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1ip63wz</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>🔮moody mani</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip63wz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1ipwef3</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Hey friends, which nail shape suits me best? 1 or 2? Thanks for your help 💙💚</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipwef3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1ipggws</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>What do you think of them? I did them</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipggws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1ipu5hg</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Frozen Nail Set</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipu5hg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1ipsrlo</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>WIP of my next Kingdom Hearts nail</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipsrlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1iprbkn</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Fresh set 🍒</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iprbkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1ipqs98</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Some practice nails I did as a beginner</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsp4y6u7k7je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1ipoiky</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>I loved them and my favorite color, red</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b505hsh6z6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1ipm8ss</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>My Valentine’s nails.</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipm8ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1ipm7qh</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>First softgel. I didn't have faith in the colors, but it turned out very beautiful 💜</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0o1y58vf6je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1ipkbmw</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Frenchies &amp; a Rose 🌹</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhdykdc216je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1ipk1jh</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Back again with two more nails done</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsfe70ruy5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1ipjvv9</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Happy Valentine's Day from me and Snoopy :p</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipjvv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1ipj1as</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Guess what am posting! (Yes it a Valentine day set ofc)</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipj1as</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1iphji5</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>My first nails with solf gel... I admit that I'm still not clear 💖</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0x0mrexf5je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1ipfvw3</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Valentine's Nails ❤️🖤</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngid6rbh35je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1ipfq3z</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Astronomical Aquarius</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b55705o925je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1ipfniz</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Barbie Loving You set - Happy Valentine everyone</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipfniz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1ipb6d4</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>I think these are my best yet…</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wlydpil724je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1ipb61p</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s day!❤️💗</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cc6ifpw724je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1ip9l07</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>I was asked for this design for a bride</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zthl2pym3je1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1ip7oc1</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>My daughter is bluey obsessed so im trying my best here....</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6y7hm12e03je1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1ip77zy</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Pretty kitty (stickers on</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ip77zy</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Feb 16 08:09:18 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_16.xlsx
+++ b/data/collected_data/2025_02_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1324"/>
+  <dimension ref="A1:C1517"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22941,6 +22941,3287 @@
         </is>
       </c>
     </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1iqmlfr</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Press on nails durability</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqmlfr/press_on_nails_durability/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1iqlcyl</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Nail Inspo</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://v.lemon8-app.com/al/OgjpdRwhNs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1iqkb29</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>First time getting nails done in 8 years!! Gel X 🥰</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqkb29</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1iqjdju</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>How can I create these nails? Inspo from @ladycrappo on tumblr</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13yqp94j9fje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1iqj41e</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Press On Recommendations?</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqj41e/press_on_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1iqmnxx</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Unsanitary tools</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqmnxx/unsanitary_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1iql9ef</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Nail Techs! E-File Recommendations?</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iql9ef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1iql4t5</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbl0p3e5sfje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1iqkij5</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>No lazy thumbs over here! 💗</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mc9my6klfje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1iqkhls</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Gel nails peeling off (at home)</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqkhls/gel_nails_peeling_off_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1iqkayk</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>My natural nails 3 weeks in gel</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxr166p9jfje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1iqk7eu</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day nails! 🖤</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45yx3hh8ifje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1iqjvi7</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Lovely French with Chrome</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqjvi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1iqjcm1</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Fresh DIY purple manicure!</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgafga799fje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1iqj0ia</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Another picture because I just love these</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pd5pf6es5fje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1iqiv8n</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>pink tips! 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jer4e1cb4fje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1iqiom9</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>nails!! I paid $85 and tipped $20 they are so so cute!!</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pw330og2fje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1iqi6hn</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Blue smiley + checkered design</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aprstc4fxeje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1iqi74e</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Sparkly red🌹</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9t3cqamlxeje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1iqi6e4</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Red, Gold &amp; Hearts 💕</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvg9uadbxeje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1iqhtgc</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>apples!!</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25vjs21yteje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1iqi21y</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Issues with builder gel- what would be better?</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqi21y/issues_with_builder_gel_what_would_be_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1iqhz9l</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Where to start?</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqhz9l/where_to_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1iqhyzf</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>red hearts french tips ❤️</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqhyzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1iqhu4g</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Kirby nail art! From Pressed Nail Bar in Cleveland</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cytawfc5ueje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1iqhf23</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Baddie on a budget💞💅🏻</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qx7j4z59qeje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1iqh9b0</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Is there a minimum amount of time I should wait between BIAB appointments?</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4blgx7tqoeje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1iqgtlq</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>How much would nails like these cost in your country?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqgtlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1iqh4ad</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Valentine's Day press-ons</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqh4ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1iqh0vr</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>🧿🧿🧿</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vw7le6ygmeje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1iqgu1c</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Getting ready for spring 💐🌷</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqgu1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1iqgs48</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>obsessed with my manicure today</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7py5y52keje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1iqg4q1</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>How to repair my peeling nail long enough to grow the damage out?</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqg4q1/how_to_repair_my_peeling_nail_long_enough_to_grow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1iqg9p4</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Tribal Black and Gold</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bj5e6bkgfeje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1iqfyy4</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Mermaid blue</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqfyy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1iqfupw</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Fresh Manicure on Natural Nails - 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqfupw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1iqfrci</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>birthday nails💗😊</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqfrci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1iqe65e</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>does anyone know how strong the glamnetic nail glue is?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqe65e/does_anyone_know_how_strong_the_glamnetic_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1iqf8rq</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Red cat eye ❣️</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gylpbouf6eje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1iqf6tv</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Shaping question</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqf6tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1iqf3uf</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Athletic glitter mani</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2aqn03d5eje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1iqex2u</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Obsessed with cat eye polishes!</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w6uz25q3eje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1iqewce</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>My first play with foils 🥲 Tips needed 😬</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hbzk63k3eje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1iqeubs</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Mylee Brown Sugar on natural nails 🤎</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqeubs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1iqet79</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Thoughts on the colour? I think I like it but i’m not sure if it suits my skin tone! 🍈</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqet79</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1iqerdm</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>First play with loose glitter 🦋 Any tips?</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqerdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1iqeqg6</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Nothing beats a red mani!💋</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqeqg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1iqepm4</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>My Autumnal set after a couple week’s wear! 🍂</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqepm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1iqeomy</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Best nail shape for tiny nail beds?</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrrwykio1eje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1iqem89</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>My Valentine’s Nails ♥️</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0t33f841eje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1iqel6v</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>My DIY Halloween set on natural nails (I know i’m late 🙈)</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkwitn3w0eje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1iqejoe</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Monday Blue by Mylee on natural nails 💙</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqejoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1iqeing</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>My first attempt at a Frenchie!</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqeing</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1iqebob</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>I envisioned this set differently than it turned out.</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ic4970xnydje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1iqe2vo</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Best top coat for non-gel?</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqe2vo/best_top_coat_for_nongel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1iqbpfm</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Why are my nails not white all the way?</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqbpfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1iqay99</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Belated Valentine’s Day Nails!</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqay99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1iqdkqj</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>My wedding nails</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yq3kqtkgsdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1iqdkc9</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Avoiding getting paint on nails</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqdkc9/avoiding_getting_paint_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1iqdhzh</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails 💅</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9wpkqfwurdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1iqdbrf</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>🪻Jelly lilac🪻</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqdbrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1iqd9ni</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>v-day nails!!</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dmcul9ypdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1iqd93s</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Valentine's Day Set 💞</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqd93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1iqd7cf</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Little Frenchie 💕</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sezlpy2gpdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1iqd5ar</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>...spring</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7x7rzyyodje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1iqcwbs</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iqcwbs/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1iqcw9a</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Different colour that I'm used to</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyewsa5zmdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1iqcumb</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>In a Brown Mood :)</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zu9qvplmdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1iqcsav</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqcsav</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1iqcr6i</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Liking this vampy color</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ounhmguldje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1iqcj6l</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkut51v2kdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1iqci0d</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>I smooshed craft glitter onto my favorite polish to brighten up this snowy day!</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqci0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1iqcfek</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>I think the dude forgot to put a top coat on one of my big toes…</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezvtnnu9jdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1iqcdm4</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Is this decent?</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqcdm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1iqc4y2</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>My V day nails!</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nr8jvgzgdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1iqap8x</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Just a guy that loves doing his own nails ☺️</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqap8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1iqaor8</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>My boy spiderman 🕷️❤️🎀</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0536k4xq5dje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1iqaeyt</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>My v-day set!</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqaeyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1iqabej</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Any tips? I do my own gel/biab</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqabej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1iqa5f7</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Clean and simple 💕</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf5k3djl1dje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1iqa2qv</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>did my vday nails</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqa2qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1iq9r13</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Mardi Gras nails 💚💛💜</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq9r13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1iq9qg1</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>I was going for a celestial Mermaid theme</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq9qg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1iq9q53</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>My valentine's day gift</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq9q53</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1iq3h69</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Left a bad review, salon’s response is making me second guess</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iq3h69/left_a_bad_review_salons_response_is_making_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1iq9ado</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Nail glue</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iq9ado/nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1iq48hj</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Cheap or stylish??</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ydse8a2rbje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1iq32v6</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Is my top coat non wipe?</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iq32v6/is_my_top_coat_non_wipe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1iq9j4x</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5n2r0c5uwcje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1iq9fnw</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>How much would you pay and tip for this?</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq9fnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1iq9c4w</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Pop of colour!</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fo0a9g9vcje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1iq80c8</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Did I get the almond shape right?</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq80c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1iq7wfh</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Birthday nails for Monday 💘</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq7wfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1iq7ds8</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>New nails! ♥️ My press-on collection is growing</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq7ds8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1iq6v3r</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Got nails done in Mexico! Recently loving cheetah print</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq6v3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1iq6p9c</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Half matte half glossy arty black nails! One of My favorite sets ever</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ju87jyqacje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1iq6dww</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>My Valentines Day gift from my Mom</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ax1aho798cje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1iq62rz</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>First time I've done a manicure, its shellac and fake nails</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq62rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1iq5o9h</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>🫧 so clean 🤍</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq5o9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1iq5fb8</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Valentine's Day manicure. Do you like the color choice?</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq5fb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1iqnc9i</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Riot Of Shadows</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqnc9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1iqmgjj</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Velvet</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqmgjj/velvet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1iqli9j</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Help me shade match my donkey</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrebit1dwfje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1iqkzu0</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>A lil late Valentine's Day set</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7utuj8mqfje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1iqip33</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Polished for Days - Smitten</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqip33</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1iqi9gx</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Post valentines palette cleanser</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyq88zqoxeje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1iqhybk</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>LynBDesigns: Aquarius (The Water Bearer) 😍</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/920ii5y8veje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1iqhvk3</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Dupe for HT Bep bep blue / matcha maker ?</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqhvk3/dupe_for_ht_bep_bep_blue_matcha_maker/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1iqhtru</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>ChromaVerse Polish: Chaos and Last Piece</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqhtru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1iqhltk</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>red heart french tips ✨</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqhltk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1iqgh0k</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Cottagecore Skittle</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqgh0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1iqfm8n</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>My first attempt to do fun designs for my wife: What tools do you lacqueristas use to do precision work?</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/be0cozln9eje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1iqfk3f</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Baby pink or milky pink</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqfk3f/baby_pink_or_milky_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1iqfgcx</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Attempt</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqfgcx/valentines_day_attempt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1iqfdmw</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>more hot pink velvet 🩷</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idoav68l7eje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1iqegl3</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Black Flake Top Coat</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqegl3/black_flake_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1iqeewa</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Birthday Nails :)</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqeewa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1iqeebi</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>New to manicures. When would you choose a gel Mani over getting gel-x?</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqeebi/new_to_manicures_when_would_you_choose_a_gel_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1iqe9qk</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>First share</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91u8t1n6ydje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1iqe5mv</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Valentine’s Mani 2025 - I’m in LOVE w/ILNP Sabrina ♥️♥️♥️</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcbxfi97xdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1iqdhiq</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Which red shimmer?  Unbreakable Will, Chicago Fire, or Redrum?</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqdhiq/which_red_shimmer_unbreakable_will_chicago_fire/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1iqddqd</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>The Little Prince</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqddqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1iqdbxz</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Proud of my length (that's what he said)</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7o1hwkfhqdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1iqd9q4</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Valentine's Day Set 💞</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqd9q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1iqd3o5</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Valentine nails</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q19nfstlodje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1iqcwjq</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>A Million Nail Care Questions from a Noob</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqcwjq/a_million_nail_care_questions_from_a_noob/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1iqclb3</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>Starlight 🌌</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uh3bckd5kdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1iqc9hy</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Tests Came Back. Positive for Cooties</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqc9hy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1iqc2bf</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Toddler nails!</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztfhlr1egdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1iqbycq</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Chipped a nail</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qym8jvrjfdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1iqbukh</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>... And Fire - Clionadh Cosmetics</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h7pceprpedje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1iqbsu0</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>First time not doing a solid color and I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lg7s7kdedje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1iqbnig</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>My valentine's color.</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkteu3x8ddje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1iqba8n</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Cuticle Softener or Remover Recommendation</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/caiyts9dadje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1iqb0mu</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Request: Mooncat - Dawn of the Empire and ILNP - Eclipse</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqb0mu/request_mooncat_dawn_of_the_empire_and_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1iqade8</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Question on layering brands</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqade8/question_on_layering_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1iqa6bz</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>I was influenced to buy this on a facebook nail group and its so fun lol</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9gs8tzps1dje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1iqa4a2</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Essie × Disney collab spotted</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqa4a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1iqa46t</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>the queen of hearts and her private jet</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqa3mp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1iq9g6a</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Swatch Req: Phoenix - You Can't Just Kill People</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iq9g6a/swatch_req_phoenix_you_cant_just_kill_people/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1iq91cf</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Cracked Haul + 2 Comparisons</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq91cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1iq8eqa</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>New fav combo just dropped 🤩</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq8eqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1iq8czl</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Bee theme</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v87203arncje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1iq84xf</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>Yesterday….all my troubles seemed so far away</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq84xf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1iq81u1</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Inocybe💚🦎🍄‍🟫🧲</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq81u1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1iq7skt</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Help me find this polish?</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq7skt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1iq73t9</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Dupe request for Olive and June's HZ Velvet? They discontinued my favorite press-ons, now I'm forced to make them myself! 😭😭</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccek1idtdcje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1iq6tt9</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>🌺Hibiscus Gradient🌺</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq6tt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1iq6rlq</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>happy vday weekend ❤️</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/heplt379bcje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1iq6qct</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>Loving the colour shift</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq6qct</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1iq6cxt</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>How would you get this kind of effect</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ay3cp6e18cje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1iq6bwc</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>When you break a nail, do you file down all your other ones to match the length of your broken nail? Or do you only file down the broken one?</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iq6bwc/when_you_break_a_nail_do_you_file_down_all_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1iq5pmi</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Vampy Valentine’s 🖤</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pbf9dbu2cje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1iq5d4i</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>Nail alternative for Elf nail polish??</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujuvq1080cje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1iq5afk</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>ILNP - Scarlett vs. EDM - All the Feelings 2.0?</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq5afk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1iq58wl</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Alternative for this polish???</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ap8894kazbje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1iq5432</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Help! Why is this happening?</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq5432</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1iq50dr</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>You can only wear one polish for one year. What brand/ color are you doing?</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://us.manucurist.com/products/green-nail-polish-gold</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1iq4na4</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Tried putting chrome over a magnetic!</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y9cyqzdeubje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1iq43hi</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>I’m only afraid of boring nails!</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u5wo62iwpbje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1iq3y77</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>valentine’s day nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r8o5b3kpobje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1iq3hgu</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Get Lobstered !!</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq3hgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1iq2ex2</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Tonight after work, I think I'm gonna try my first ever magnetic polish! Please give me tips!</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iq2ex2/tonight_after_work_i_think_im_gonna_try_my_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1iq1sdm</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Help - one of my bottles isn't opening. Product leak and it's now completely dried up rock solid.</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucgcfxox5bje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1iq1nyq</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>Tried to do a vertical cat eye which worked in my head but definitely not irl!</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/glqyrtzg4bje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1iq155e</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Making a blood red jelly / sheer polish at home?</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iq155e/making_a_blood_red_jelly_sheer_polish_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1iq0vde</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Magnet stand/holder recommendations?</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iq0vde/magnet_standholder_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1ipzqvm</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>One of my new favorite purples 💜</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipzqvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1ipygkq</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Beachy/summery vibes 🌊 (Originally by @e.bee_nails on insta)</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sin6cf33aje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1ipy4ef</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>Phoenix Bill is 🔥</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipy4ef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1ipxprq</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>Glisten &amp; Glow top coat</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ipxprq/glisten_glow_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1ipmwzq</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>I think I found a new fav??</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipmwzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1iqmmum</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>🙃</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pw5idhk9gje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1iqljz5</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Off theme valentines nails</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqljz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1iqlfmi</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>Lovesick</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqlfmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1iqkwd1</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>Worked all week before Valentine's Day so these are a lil late ❤️💖</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nu28pd0lpfje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>1iqkgy7</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>treasure dreams ✨🌈</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqkgy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>1iqh2zl</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>Late Valentines Nail Art Post</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4chqw91neje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>1iqfrks</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Severance 📊</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/juiv2t5waeje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>1iqchz5</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>*Late* Valentine’s Day Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iqchz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>1iqc0v2</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>Before/after</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp32o5i2gdje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>1iqal5a</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>Two layer polish</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iqal5a/two_layer_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>1iq8p19</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>Mitsuri Nails!</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq8p19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>1iq77vx</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>Nails done by myself for valentine's</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/naz4b5brecje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>1iq52li</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>It's giving vintage</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enngt41vxbje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>1iq4wfg</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>Black and red</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n01rz0tewbje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>1iq4twe</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>New nails I made!</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgg1qn5vvbje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>1iq4ryw</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>Lace set</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oxly2j3fvbje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>1iq4py2</t>
+        </is>
+      </c>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>Space alien girly nail set</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iq4py2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>1iq33cv</t>
+        </is>
+      </c>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>Is my top coat non wipe?</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iq33cv/is_my_top_coat_non_wipe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>1ipzyd0</t>
+        </is>
+      </c>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>New press on set! I’m a beginner</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ipzyd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>1ipz686</t>
+        </is>
+      </c>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>These little works of art took me a total of 5 hours, I hand painted everything myself</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rq5f51okcaje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr">
+        <is>
+          <t>1ipz4xk</t>
+        </is>
+      </c>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>my nail art for valentine's day</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhw5iqb3caje1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>